<commit_message>
reupdate missing class and fix class issues
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kavya.mothukuri/workspace/SeleniumAutomation/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16335" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
     <sheet name="FirstSet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>dev</t>
   </si>
@@ -115,13 +110,16 @@
   </si>
   <si>
     <t>IntakeMgr</t>
+  </si>
+  <si>
+    <t>intake.user1@cvhcare.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -255,7 +253,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -432,24 +430,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -457,7 +455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -465,17 +463,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -486,20 +484,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.375" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -510,7 +508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -521,7 +519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -532,7 +530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,93 +541,100 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1"/>
       <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1"/>
       <c r="C6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="C8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="C9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="C11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="C12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="C14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="C15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="C16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3">
       <c r="C17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3">
       <c r="C18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:3">
       <c r="C19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:3">
       <c r="C20" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new test case for Profile settings. Current qa.test1@cvhcare.com password is Password2!
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>dev</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>intake.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>Password2!</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,7 +516,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
update for scheduling testcase
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>dev</t>
   </si>
@@ -119,6 +119,39 @@
   </si>
   <si>
     <t>scheduler.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>clinician.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>schedulermanager.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>clinicianmanager.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>auditor.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>auditormanager.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>authz.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>authzmanager.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>order.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>ordermanager.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>cq.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>cqmanager.user1@cvhcare.com</t>
   </si>
 </sst>
 </file>
@@ -436,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,7 +527,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -549,12 +582,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -571,6 +610,9 @@
       </c>
     </row>
     <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
@@ -587,56 +629,122 @@
       </c>
     </row>
     <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="3:3">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
       <c r="C19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
@@ -648,6 +756,17 @@
     <hyperlink ref="A2" r:id="rId3"/>
     <hyperlink ref="A7" r:id="rId4"/>
     <hyperlink ref="A9" r:id="rId5"/>
+    <hyperlink ref="A11" r:id="rId6"/>
+    <hyperlink ref="A10" r:id="rId7"/>
+    <hyperlink ref="A12" r:id="rId8"/>
+    <hyperlink ref="A13" r:id="rId9"/>
+    <hyperlink ref="A14" r:id="rId10"/>
+    <hyperlink ref="A15" r:id="rId11"/>
+    <hyperlink ref="A16" r:id="rId12"/>
+    <hyperlink ref="A17" r:id="rId13"/>
+    <hyperlink ref="A18" r:id="rId14"/>
+    <hyperlink ref="A19" r:id="rId15"/>
+    <hyperlink ref="A20" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
stage but not yet merge
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -112,9 +112,6 @@
     <t>intake.user1@cvhcare.com</t>
   </si>
   <si>
-    <t>Password2!</t>
-  </si>
-  <si>
     <t>scheduler.user1@cvhcare.com</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>clinician.user3@cvhcare.com</t>
+  </si>
+  <si>
+    <t>Password0!</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,7 +524,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -549,7 +549,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
scheduling anf part clinician
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>dev</t>
   </si>
@@ -112,12 +112,6 @@
     <t>intake.user1@cvhcare.com</t>
   </si>
   <si>
-    <t>scheduler.user1@cvhcare.com</t>
-  </si>
-  <si>
-    <t>schedulermanager.user1@cvhcare.com</t>
-  </si>
-  <si>
     <t>clinicianmanager.user1@cvhcare.com</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>clinician.user3@cvhcare.com</t>
   </si>
   <si>
-    <t>Password0!</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>hr.user1@cvhcare.com</t>
   </si>
   <si>
-    <t>clinician.pt1@cvhcare.com</t>
-  </si>
-  <si>
     <t>PT</t>
   </si>
   <si>
@@ -172,7 +160,13 @@
     <t>marc.miller@cvhcare.com</t>
   </si>
   <si>
-    <t>cvhcare.admin@cvhcare.com</t>
+    <t>qa@cvhcare.com</t>
+  </si>
+  <si>
+    <t>kavya.mothukuri@cvhcare.com</t>
+  </si>
+  <si>
+    <t>russell.sadang@cvhcare.com</t>
   </si>
 </sst>
 </file>
@@ -490,7 +484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,7 +542,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -570,10 +564,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -629,7 +623,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -640,7 +634,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -651,7 +645,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -662,7 +656,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -673,7 +667,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -684,7 +678,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -695,7 +689,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -706,7 +700,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -717,7 +711,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -728,7 +722,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -739,7 +733,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -750,7 +744,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -761,46 +755,46 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -808,22 +802,22 @@
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A6" r:id="rId3"/>
-    <hyperlink ref="A8" r:id="rId4"/>
-    <hyperlink ref="A9" r:id="rId5"/>
-    <hyperlink ref="A11" r:id="rId6"/>
-    <hyperlink ref="A12" r:id="rId7"/>
-    <hyperlink ref="A13" r:id="rId8"/>
-    <hyperlink ref="A14" r:id="rId9"/>
-    <hyperlink ref="A15" r:id="rId10"/>
-    <hyperlink ref="A16" r:id="rId11"/>
-    <hyperlink ref="A17" r:id="rId12"/>
-    <hyperlink ref="A18" r:id="rId13"/>
-    <hyperlink ref="A19" r:id="rId14"/>
-    <hyperlink ref="A10" r:id="rId15"/>
-    <hyperlink ref="A20" r:id="rId16"/>
-    <hyperlink ref="A21" r:id="rId17"/>
-    <hyperlink ref="A22" r:id="rId18"/>
-    <hyperlink ref="A23" r:id="rId19"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="A11" r:id="rId5"/>
+    <hyperlink ref="A12" r:id="rId6"/>
+    <hyperlink ref="A13" r:id="rId7"/>
+    <hyperlink ref="A14" r:id="rId8"/>
+    <hyperlink ref="A15" r:id="rId9"/>
+    <hyperlink ref="A16" r:id="rId10"/>
+    <hyperlink ref="A17" r:id="rId11"/>
+    <hyperlink ref="A18" r:id="rId12"/>
+    <hyperlink ref="A19" r:id="rId13"/>
+    <hyperlink ref="A10" r:id="rId14"/>
+    <hyperlink ref="A20" r:id="rId15"/>
+    <hyperlink ref="A21" r:id="rId16"/>
+    <hyperlink ref="A22" r:id="rId17"/>
+    <hyperlink ref="A23" r:id="rId18"/>
+    <hyperlink ref="A8" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>

</xml_diff>

<commit_message>
fix for profile password account
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -106,9 +106,6 @@
     <t>IntakeMgr</t>
   </si>
   <si>
-    <t>auditormanager.user1@cvhcare.com</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>jamey.dixon@cvhcare.com</t>
+  </si>
+  <si>
+    <t>Lisa.Edwards@cvhcare.com</t>
   </si>
 </sst>
 </file>
@@ -223,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -231,6 +231,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -502,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -560,7 +563,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -582,10 +585,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -593,10 +596,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -604,10 +607,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -615,10 +618,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -626,10 +629,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -637,10 +640,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -648,10 +651,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -659,10 +662,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -670,10 +673,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -681,10 +684,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -692,10 +695,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -703,10 +706,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -714,10 +717,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -725,10 +728,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -736,10 +739,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -747,10 +750,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -758,10 +761,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
@@ -769,10 +772,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -780,156 +783,156 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>27</v>
+      <c r="A25" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
         <v>43</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -960,8 +963,9 @@
     <hyperlink ref="A22" r:id="rId24"/>
     <hyperlink ref="A23" r:id="rId25"/>
     <hyperlink ref="A24" r:id="rId26"/>
+    <hyperlink ref="A25" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated clinician test data.
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -151,38 +151,38 @@
     <t>qateam</t>
   </si>
   <si>
-    <t>alia.dolan@cvhcare.com</t>
-  </si>
-  <si>
-    <t>alison.burton@cvhcare.com</t>
-  </si>
-  <si>
-    <t>chioma.okpara@cvhcare.com</t>
-  </si>
-  <si>
-    <t>amanda.walters@cvhcare.com</t>
-  </si>
-  <si>
-    <t>elsie.szeto@cvhcare.com</t>
-  </si>
-  <si>
-    <t>aaron.gatuz@cvhcare.com</t>
-  </si>
-  <si>
-    <t>jamey.dixon@cvhcare.com</t>
-  </si>
-  <si>
     <t>Lisa.Edwards@cvhcare.com</t>
   </si>
   <si>
     <t>test.qa@cvhcare.com</t>
+  </si>
+  <si>
+    <t>test_pt@cvhcare.com</t>
+  </si>
+  <si>
+    <t>test_rn@cvhcare.com</t>
+  </si>
+  <si>
+    <t>test_msw@cvhcare.com</t>
+  </si>
+  <si>
+    <t>test_chha@cvhcare.com</t>
+  </si>
+  <si>
+    <t>test_ot@cvhcare.com</t>
+  </si>
+  <si>
+    <t>test_rd@cvhcare.com</t>
+  </si>
+  <si>
+    <t>test_st@cvhcare.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,6 +197,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,18 +227,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -502,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -559,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -582,7 +584,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -593,7 +595,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -604,7 +606,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -615,7 +617,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -626,7 +628,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -637,7 +639,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -648,7 +650,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -659,7 +661,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -670,7 +672,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -681,7 +683,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -692,7 +694,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -703,7 +705,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -714,7 +716,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -725,7 +727,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -736,7 +738,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -747,7 +749,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -758,7 +760,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -769,7 +771,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -780,7 +782,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -791,7 +793,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -802,7 +804,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -813,7 +815,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -824,7 +826,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -834,8 +836,8 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4" t="s">
-        <v>49</v>
+      <c r="A25" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -845,8 +847,8 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
-        <v>47</v>
+      <c r="A26" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -856,8 +858,8 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2" t="s">
-        <v>43</v>
+      <c r="A27" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -867,8 +869,8 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>42</v>
+      <c r="A28" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -878,8 +880,8 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
-        <v>44</v>
+      <c r="A29" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -889,8 +891,8 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
-        <v>45</v>
+      <c r="A30" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -901,7 +903,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -911,8 +913,8 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2" t="s">
-        <v>48</v>
+      <c r="A32" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -923,7 +925,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -935,34 +937,39 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A33" r:id="rId1" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A30" r:id="rId2"/>
-    <hyperlink ref="A31" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A3" r:id="rId5" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A4" r:id="rId6" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A5" r:id="rId7" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A6" r:id="rId8" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A7" r:id="rId9" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A8" r:id="rId10" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A9" r:id="rId11" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A10" r:id="rId12" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A11" r:id="rId13" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A12" r:id="rId14" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A13" r:id="rId15" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A14" r:id="rId16" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A15" r:id="rId17" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A16" r:id="rId18" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A17" r:id="rId19" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A18" r:id="rId20" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A19" r:id="rId21" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A20" r:id="rId22" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A21" r:id="rId23" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A22" r:id="rId24" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A23" r:id="rId25" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A24" r:id="rId26" display="kavya.mothukuri@cvhcare.com"/>
-    <hyperlink ref="A25" r:id="rId27"/>
+    <hyperlink ref="A2" r:id="rId2" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A4" r:id="rId4" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A5" r:id="rId5" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A6" r:id="rId6" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A7" r:id="rId7" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A8" r:id="rId8" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A9" r:id="rId9" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A10" r:id="rId10" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A11" r:id="rId11" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A12" r:id="rId12" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A13" r:id="rId13" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A14" r:id="rId14" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A15" r:id="rId15" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A16" r:id="rId16" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A17" r:id="rId17" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A18" r:id="rId18" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A19" r:id="rId19" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A20" r:id="rId20" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A21" r:id="rId21" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A22" r:id="rId22" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A23" r:id="rId23" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A24" r:id="rId24" display="kavya.mothukuri@cvhcare.com"/>
+    <hyperlink ref="A25" r:id="rId25"/>
+    <hyperlink ref="A26" r:id="rId26"/>
+    <hyperlink ref="A27" r:id="rId27"/>
+    <hyperlink ref="A28" r:id="rId28"/>
+    <hyperlink ref="A29" r:id="rId29"/>
+    <hyperlink ref="A30" r:id="rId30"/>
+    <hyperlink ref="A31" r:id="rId31"/>
+    <hyperlink ref="A32" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>